<commit_message>
fix skills column names
</commit_message>
<xml_diff>
--- a/data/atr_data.xlsx
+++ b/data/atr_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pp-brandon/Projects/uiowa-atr/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2611214C-341A-BB43-B90F-01A3CC3F9B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B15CF98-E6CB-B446-ADF0-C9680DDA201A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,12 +637,6 @@
     <t>Helpful videos that range from listening games such as “Guess the sound,” these can include animal, household, or environmental sounds. Some videos also include instructions for parents to conduct listening activities with their children. Most are aimed at children rather than adults but can be utilized for both. </t>
   </si>
   <si>
-    <t>BACKGROUND NOISE OPTION</t>
-  </si>
-  <si>
-    <t>ENVIRONMENTAL SOUNDS</t>
-  </si>
-  <si>
     <t>Cochlear Americas</t>
   </si>
   <si>
@@ -659,6 +653,12 @@
   </si>
   <si>
     <t>seeing_and_hearing_speech.png</t>
+  </si>
+  <si>
+    <t>BACKGROUND</t>
+  </si>
+  <si>
+    <t>ENVIRONMENT</t>
   </si>
 </sst>
 </file>
@@ -1242,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1254,9 +1254,12 @@
     <col min="4" max="4" width="10.5" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.83203125" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="14" max="14" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.83203125" customWidth="1"/>
+    <col min="17" max="17" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="21.33203125" customWidth="1"/>
     <col min="19" max="19" width="8.6640625" customWidth="1"/>
     <col min="20" max="20" width="11.6640625" customWidth="1"/>
@@ -1332,7 +1335,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>16</v>
@@ -1350,7 +1353,7 @@
         <v>20</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="O2" s="8" t="s">
         <v>21</v>
@@ -1456,7 +1459,7 @@
         <v>30</v>
       </c>
       <c r="R4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="T4" t="s">
         <v>30</v>
@@ -1769,7 +1772,7 @@
         <v>30</v>
       </c>
       <c r="R12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="S12" s="13"/>
       <c r="T12" t="s">
@@ -1808,7 +1811,7 @@
         <v>30</v>
       </c>
       <c r="R13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="S13" s="13" t="s">
         <v>30</v>
@@ -1855,7 +1858,7 @@
         <v>30</v>
       </c>
       <c r="R14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="S14" s="13" t="s">
         <v>30</v>
@@ -2040,7 +2043,7 @@
         <v>30</v>
       </c>
       <c r="R18" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="U18" t="s">
         <v>30</v>
@@ -2271,7 +2274,7 @@
         <v>133</v>
       </c>
       <c r="X24" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
@@ -2312,7 +2315,7 @@
         <v>30</v>
       </c>
       <c r="W25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="X25" s="12" t="s">
         <v>137</v>
@@ -2450,7 +2453,7 @@
         <v>133</v>
       </c>
       <c r="X28" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
@@ -2538,7 +2541,7 @@
         <v>133</v>
       </c>
       <c r="X30" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
upload base_template and remove another unsupported resource
</commit_message>
<xml_diff>
--- a/data/atr_data.xlsx
+++ b/data/atr_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pp-brandon/Projects/uiowa-atr/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B15CF98-E6CB-B446-ADF0-C9680DDA201A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0472EE8-5DBB-C44A-B044-C7676E906E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="181">
   <si>
     <t>Resource:</t>
   </si>
@@ -220,21 +220,6 @@
   </si>
   <si>
     <t>App made mainly for listening to audiobooks, also includes podcasts. Can be used for CI users’ needing more advanced listening practice. </t>
-  </si>
-  <si>
-    <t>Auditory Skills Checklist</t>
-  </si>
-  <si>
-    <t>https://apps.apple.com/us/app/auditory-skills-checklist/id1111515267</t>
-  </si>
-  <si>
-    <t>https://play.google.com/store/apps/details?id=com.medel.auditory&amp;hl=en_US&amp;gl=US</t>
-  </si>
-  <si>
-    <t>auditory_skills_checklist.webp</t>
-  </si>
-  <si>
-    <t>Application that can be used to establish goals and/or track progress made in different auditory areas. Checklist uses multiple choice questions to determine if a child has responded using auditory cues/auditory information. Most appropriate for parents or caregivers to use for children. Good to use to monitor over time. </t>
   </si>
   <si>
     <t>BabyBeats</t>
@@ -1240,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X34"/>
+  <dimension ref="A1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1335,7 +1320,7 @@
         <v>15</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>16</v>
@@ -1353,7 +1338,7 @@
         <v>20</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="O2" s="8" t="s">
         <v>21</v>
@@ -1459,7 +1444,7 @@
         <v>30</v>
       </c>
       <c r="R4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="T4" t="s">
         <v>30</v>
@@ -1693,13 +1678,19 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>100</v>
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" t="s">
+        <v>30</v>
       </c>
       <c r="O10" t="s">
         <v>30</v>
       </c>
       <c r="R10" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="T10" t="s">
         <v>30</v>
@@ -1718,70 +1709,73 @@
       <c r="B11" t="s">
         <v>71</v>
       </c>
-      <c r="C11" t="s">
-        <v>72</v>
-      </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>10</v>
-      </c>
-      <c r="H11" t="s">
-        <v>30</v>
-      </c>
-      <c r="M11" t="s">
+        <v>100</v>
+      </c>
+      <c r="J11" t="s">
         <v>30</v>
       </c>
       <c r="O11" t="s">
         <v>30</v>
       </c>
+      <c r="P11" t="s">
+        <v>30</v>
+      </c>
       <c r="R11" t="s">
-        <v>31</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="S11" s="13"/>
       <c r="T11" t="s">
         <v>30</v>
       </c>
       <c r="W11" t="s">
+        <v>72</v>
+      </c>
+      <c r="X11" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="X11" s="12" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
         <v>75</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>76</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G12">
         <v>100</v>
       </c>
-      <c r="J12" t="s">
-        <v>30</v>
-      </c>
-      <c r="O12" t="s">
+      <c r="M12" t="s">
         <v>30</v>
       </c>
       <c r="P12" t="s">
         <v>30</v>
       </c>
+      <c r="Q12" t="s">
+        <v>30</v>
+      </c>
       <c r="R12" t="s">
-        <v>182</v>
-      </c>
-      <c r="S12" s="13"/>
+        <v>173</v>
+      </c>
+      <c r="S12" s="13" t="s">
+        <v>30</v>
+      </c>
       <c r="T12" t="s">
         <v>30</v>
       </c>
       <c r="W12" t="s">
         <v>77</v>
       </c>
-      <c r="X12" s="12" t="s">
+      <c r="X12" s="14" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1792,26 +1786,32 @@
       <c r="B13" t="s">
         <v>80</v>
       </c>
-      <c r="C13" t="s">
-        <v>81</v>
-      </c>
       <c r="F13">
         <v>10</v>
       </c>
       <c r="G13">
         <v>100</v>
       </c>
-      <c r="M13" t="s">
+      <c r="H13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" t="s">
         <v>30</v>
       </c>
       <c r="P13" t="s">
         <v>30</v>
       </c>
-      <c r="Q13" t="s">
-        <v>30</v>
-      </c>
       <c r="R13" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="S13" s="13" t="s">
         <v>30</v>
@@ -1820,21 +1820,24 @@
         <v>30</v>
       </c>
       <c r="W13" t="s">
+        <v>81</v>
+      </c>
+      <c r="X13" s="14" t="s">
         <v>82</v>
-      </c>
-      <c r="X13" s="14" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" t="s">
         <v>84</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>85</v>
       </c>
       <c r="F14">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>100</v>
@@ -1842,6 +1845,9 @@
       <c r="H14" t="s">
         <v>30</v>
       </c>
+      <c r="I14" t="s">
+        <v>30</v>
+      </c>
       <c r="J14" t="s">
         <v>30</v>
       </c>
@@ -1851,40 +1857,46 @@
       <c r="L14" t="s">
         <v>30</v>
       </c>
+      <c r="M14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" t="s">
+        <v>30</v>
+      </c>
       <c r="O14" t="s">
         <v>30</v>
       </c>
       <c r="P14" t="s">
         <v>30</v>
       </c>
+      <c r="Q14" t="s">
+        <v>30</v>
+      </c>
       <c r="R14" t="s">
-        <v>178</v>
-      </c>
-      <c r="S14" s="13" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="T14" t="s">
         <v>30</v>
       </c>
       <c r="W14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="X14" s="14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G15">
         <v>100</v>
@@ -1892,72 +1904,57 @@
       <c r="H15" t="s">
         <v>30</v>
       </c>
-      <c r="I15" t="s">
-        <v>30</v>
-      </c>
       <c r="J15" t="s">
         <v>30</v>
       </c>
-      <c r="K15" t="s">
-        <v>30</v>
-      </c>
-      <c r="L15" t="s">
-        <v>30</v>
-      </c>
       <c r="M15" t="s">
         <v>30</v>
       </c>
       <c r="N15" t="s">
         <v>30</v>
       </c>
-      <c r="O15" t="s">
-        <v>30</v>
-      </c>
-      <c r="P15" t="s">
-        <v>30</v>
-      </c>
       <c r="Q15" t="s">
         <v>30</v>
       </c>
       <c r="R15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="T15" t="s">
         <v>30</v>
       </c>
+      <c r="U15" t="s">
+        <v>30</v>
+      </c>
       <c r="W15" t="s">
-        <v>92</v>
-      </c>
-      <c r="X15" s="14" t="s">
         <v>93</v>
+      </c>
+      <c r="X15" s="12" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B16" t="s">
         <v>95</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>96</v>
       </c>
       <c r="F16">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>100</v>
-      </c>
-      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
         <v>30</v>
       </c>
       <c r="J16" t="s">
         <v>30</v>
       </c>
-      <c r="M16" t="s">
-        <v>30</v>
-      </c>
-      <c r="N16" t="s">
+      <c r="K16" t="s">
+        <v>30</v>
+      </c>
+      <c r="P16" t="s">
         <v>30</v>
       </c>
       <c r="Q16" t="s">
@@ -1965,9 +1962,6 @@
       </c>
       <c r="R16" t="s">
         <v>97</v>
-      </c>
-      <c r="T16" t="s">
-        <v>30</v>
       </c>
       <c r="U16" t="s">
         <v>30</v>
@@ -1983,22 +1977,16 @@
       <c r="A17" t="s">
         <v>100</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>101</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G17">
-        <v>10</v>
-      </c>
-      <c r="I17" t="s">
-        <v>30</v>
-      </c>
-      <c r="J17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K17" t="s">
+        <v>100</v>
+      </c>
+      <c r="M17" t="s">
         <v>30</v>
       </c>
       <c r="P17" t="s">
@@ -2008,24 +1996,24 @@
         <v>30</v>
       </c>
       <c r="R17" t="s">
+        <v>173</v>
+      </c>
+      <c r="U17" t="s">
+        <v>30</v>
+      </c>
+      <c r="W17" t="s">
+        <v>37</v>
+      </c>
+      <c r="X17" s="12" t="s">
         <v>102</v>
-      </c>
-      <c r="U17" t="s">
-        <v>30</v>
-      </c>
-      <c r="W17" t="s">
-        <v>103</v>
-      </c>
-      <c r="X17" s="12" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>105</v>
-      </c>
-      <c r="E18" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+      <c r="D18" t="s">
+        <v>104</v>
       </c>
       <c r="F18">
         <v>10</v>
@@ -2033,60 +2021,60 @@
       <c r="G18">
         <v>100</v>
       </c>
-      <c r="M18" t="s">
-        <v>30</v>
-      </c>
-      <c r="P18" t="s">
+      <c r="J18" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" t="s">
+        <v>30</v>
+      </c>
+      <c r="N18" t="s">
         <v>30</v>
       </c>
       <c r="Q18" t="s">
         <v>30</v>
       </c>
       <c r="R18" t="s">
-        <v>178</v>
+        <v>103</v>
       </c>
       <c r="U18" t="s">
         <v>30</v>
       </c>
       <c r="W18" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="X18" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B19" t="s">
         <v>108</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>10</v>
+      </c>
+      <c r="K19" t="s">
+        <v>30</v>
+      </c>
+      <c r="P19" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>30</v>
+      </c>
+      <c r="R19" t="s">
         <v>109</v>
       </c>
-      <c r="F19">
-        <v>10</v>
-      </c>
-      <c r="G19">
-        <v>100</v>
-      </c>
-      <c r="J19" t="s">
-        <v>30</v>
-      </c>
-      <c r="K19" t="s">
-        <v>30</v>
-      </c>
-      <c r="L19" t="s">
-        <v>30</v>
-      </c>
-      <c r="N19" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>30</v>
-      </c>
-      <c r="R19" t="s">
-        <v>108</v>
-      </c>
-      <c r="U19" t="s">
+      <c r="T19" t="s">
         <v>30</v>
       </c>
       <c r="W19" t="s">
@@ -2100,7 +2088,7 @@
       <c r="A20" t="s">
         <v>112</v>
       </c>
-      <c r="B20" t="s">
+      <c r="E20" t="s">
         <v>113</v>
       </c>
       <c r="F20">
@@ -2109,74 +2097,77 @@
       <c r="G20">
         <v>10</v>
       </c>
+      <c r="J20" t="s">
+        <v>30</v>
+      </c>
       <c r="K20" t="s">
         <v>30</v>
       </c>
+      <c r="O20" t="s">
+        <v>30</v>
+      </c>
       <c r="P20" t="s">
         <v>30</v>
       </c>
-      <c r="Q20" t="s">
-        <v>30</v>
-      </c>
       <c r="R20" t="s">
+        <v>55</v>
+      </c>
+      <c r="T20" t="s">
+        <v>30</v>
+      </c>
+      <c r="W20" t="s">
+        <v>56</v>
+      </c>
+      <c r="X20" s="12" t="s">
         <v>114</v>
-      </c>
-      <c r="T20" t="s">
-        <v>30</v>
-      </c>
-      <c r="W20" t="s">
-        <v>115</v>
-      </c>
-      <c r="X20" s="12" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" t="s">
         <v>117</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
+      <c r="M21" t="s">
+        <v>30</v>
+      </c>
+      <c r="O21" t="s">
+        <v>30</v>
+      </c>
+      <c r="P21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>30</v>
+      </c>
+      <c r="R21" t="s">
         <v>118</v>
       </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>10</v>
-      </c>
-      <c r="J21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K21" t="s">
-        <v>30</v>
-      </c>
-      <c r="O21" t="s">
-        <v>30</v>
-      </c>
-      <c r="P21" t="s">
-        <v>30</v>
-      </c>
-      <c r="R21" t="s">
-        <v>55</v>
-      </c>
       <c r="T21" t="s">
         <v>30</v>
       </c>
       <c r="W21" t="s">
-        <v>56</v>
+        <v>119</v>
       </c>
       <c r="X21" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B22" t="s">
-        <v>121</v>
-      </c>
-      <c r="C22" t="s">
         <v>122</v>
       </c>
       <c r="F22">
@@ -2185,23 +2176,14 @@
       <c r="G22">
         <v>100</v>
       </c>
-      <c r="M22" t="s">
-        <v>30</v>
-      </c>
-      <c r="O22" t="s">
-        <v>30</v>
-      </c>
-      <c r="P22" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q22" t="s">
+      <c r="J22" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" t="s">
         <v>30</v>
       </c>
       <c r="R22" t="s">
         <v>123</v>
-      </c>
-      <c r="T22" t="s">
-        <v>30</v>
       </c>
       <c r="W22" t="s">
         <v>124</v>
@@ -2214,7 +2196,7 @@
       <c r="A23" t="s">
         <v>126</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>127</v>
       </c>
       <c r="F23">
@@ -2223,28 +2205,37 @@
       <c r="G23">
         <v>100</v>
       </c>
-      <c r="J23" t="s">
-        <v>30</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="M23" t="s">
+        <v>30</v>
+      </c>
+      <c r="O23" t="s">
+        <v>30</v>
+      </c>
+      <c r="P23" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q23" t="s">
         <v>30</v>
       </c>
       <c r="R23" t="s">
+        <v>31</v>
+      </c>
+      <c r="T23" t="s">
+        <v>30</v>
+      </c>
+      <c r="W23" t="s">
         <v>128</v>
       </c>
-      <c r="W23" t="s">
-        <v>129</v>
-      </c>
       <c r="X23" s="12" t="s">
-        <v>130</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F24">
         <v>10</v>
@@ -2252,10 +2243,16 @@
       <c r="G24">
         <v>100</v>
       </c>
-      <c r="M24" t="s">
-        <v>30</v>
-      </c>
-      <c r="O24" t="s">
+      <c r="I24" t="s">
+        <v>30</v>
+      </c>
+      <c r="J24" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" t="s">
+        <v>30</v>
+      </c>
+      <c r="N24" t="s">
         <v>30</v>
       </c>
       <c r="P24" t="s">
@@ -2265,24 +2262,24 @@
         <v>30</v>
       </c>
       <c r="R24" t="s">
-        <v>31</v>
-      </c>
-      <c r="T24" t="s">
+        <v>131</v>
+      </c>
+      <c r="U24" t="s">
         <v>30</v>
       </c>
       <c r="W24" t="s">
-        <v>133</v>
+        <v>178</v>
       </c>
       <c r="X24" s="12" t="s">
-        <v>181</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" t="s">
         <v>134</v>
-      </c>
-      <c r="D25" t="s">
-        <v>135</v>
       </c>
       <c r="F25">
         <v>10</v>
@@ -2299,9 +2296,15 @@
       <c r="K25" t="s">
         <v>30</v>
       </c>
+      <c r="L25" t="s">
+        <v>30</v>
+      </c>
       <c r="N25" t="s">
         <v>30</v>
       </c>
+      <c r="O25" t="s">
+        <v>30</v>
+      </c>
       <c r="P25" t="s">
         <v>30</v>
       </c>
@@ -2309,15 +2312,18 @@
         <v>30</v>
       </c>
       <c r="R25" t="s">
+        <v>135</v>
+      </c>
+      <c r="T25" t="s">
+        <v>30</v>
+      </c>
+      <c r="U25" t="s">
+        <v>30</v>
+      </c>
+      <c r="W25" t="s">
         <v>136</v>
       </c>
-      <c r="U25" t="s">
-        <v>30</v>
-      </c>
-      <c r="W25" t="s">
-        <v>183</v>
-      </c>
-      <c r="X25" s="12" t="s">
+      <c r="X25" s="14" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2328,38 +2334,23 @@
       <c r="B26" t="s">
         <v>139</v>
       </c>
+      <c r="C26" t="s">
+        <v>140</v>
+      </c>
+      <c r="D26" t="s">
+        <v>141</v>
+      </c>
       <c r="F26">
         <v>10</v>
       </c>
       <c r="G26">
         <v>100</v>
       </c>
-      <c r="I26" t="s">
-        <v>30</v>
-      </c>
-      <c r="J26" t="s">
-        <v>30</v>
-      </c>
-      <c r="K26" t="s">
-        <v>30</v>
-      </c>
-      <c r="L26" t="s">
-        <v>30</v>
-      </c>
-      <c r="N26" t="s">
-        <v>30</v>
-      </c>
-      <c r="O26" t="s">
-        <v>30</v>
-      </c>
-      <c r="P26" t="s">
-        <v>30</v>
-      </c>
       <c r="Q26" t="s">
         <v>30</v>
       </c>
       <c r="R26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="T26" t="s">
         <v>30</v>
@@ -2368,24 +2359,18 @@
         <v>30</v>
       </c>
       <c r="W26" t="s">
-        <v>141</v>
-      </c>
-      <c r="X26" s="14" t="s">
         <v>142</v>
+      </c>
+      <c r="X26" s="12" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>143</v>
-      </c>
-      <c r="B27" t="s">
         <v>144</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>145</v>
-      </c>
-      <c r="D27" t="s">
-        <v>146</v>
       </c>
       <c r="F27">
         <v>10</v>
@@ -2393,31 +2378,43 @@
       <c r="G27">
         <v>100</v>
       </c>
+      <c r="K27" t="s">
+        <v>30</v>
+      </c>
+      <c r="L27" t="s">
+        <v>30</v>
+      </c>
+      <c r="N27" t="s">
+        <v>30</v>
+      </c>
+      <c r="O27" t="s">
+        <v>30</v>
+      </c>
+      <c r="P27" t="s">
+        <v>30</v>
+      </c>
       <c r="Q27" t="s">
         <v>30</v>
       </c>
       <c r="R27" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="T27" t="s">
         <v>30</v>
       </c>
-      <c r="U27" t="s">
-        <v>30</v>
-      </c>
       <c r="W27" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="X27" s="12" t="s">
-        <v>148</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>149</v>
-      </c>
-      <c r="D28" t="s">
-        <v>150</v>
+        <v>146</v>
+      </c>
+      <c r="B28" t="s">
+        <v>147</v>
       </c>
       <c r="F28">
         <v>10</v>
@@ -2428,15 +2425,9 @@
       <c r="K28" t="s">
         <v>30</v>
       </c>
-      <c r="L28" t="s">
-        <v>30</v>
-      </c>
       <c r="N28" t="s">
         <v>30</v>
       </c>
-      <c r="O28" t="s">
-        <v>30</v>
-      </c>
       <c r="P28" t="s">
         <v>30</v>
       </c>
@@ -2444,23 +2435,23 @@
         <v>30</v>
       </c>
       <c r="R28" t="s">
-        <v>31</v>
+        <v>148</v>
       </c>
       <c r="T28" t="s">
         <v>30</v>
       </c>
       <c r="W28" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="X28" s="12" t="s">
-        <v>179</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>151</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
         <v>152</v>
       </c>
       <c r="F29">
@@ -2469,10 +2460,22 @@
       <c r="G29">
         <v>100</v>
       </c>
+      <c r="I29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J29" t="s">
+        <v>30</v>
+      </c>
       <c r="K29" t="s">
         <v>30</v>
       </c>
-      <c r="N29" t="s">
+      <c r="L29" t="s">
+        <v>30</v>
+      </c>
+      <c r="M29" t="s">
+        <v>30</v>
+      </c>
+      <c r="O29" t="s">
         <v>30</v>
       </c>
       <c r="P29" t="s">
@@ -2482,24 +2485,24 @@
         <v>30</v>
       </c>
       <c r="R29" t="s">
-        <v>153</v>
+        <v>31</v>
       </c>
       <c r="T29" t="s">
         <v>30</v>
       </c>
       <c r="W29" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="X29" s="12" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>156</v>
-      </c>
-      <c r="D30" t="s">
-        <v>157</v>
+        <v>153</v>
+      </c>
+      <c r="C30" t="s">
+        <v>154</v>
       </c>
       <c r="F30">
         <v>10</v>
@@ -2507,55 +2510,40 @@
       <c r="G30">
         <v>100</v>
       </c>
-      <c r="I30" t="s">
-        <v>30</v>
-      </c>
-      <c r="J30" t="s">
-        <v>30</v>
-      </c>
       <c r="K30" t="s">
         <v>30</v>
       </c>
       <c r="L30" t="s">
         <v>30</v>
       </c>
-      <c r="M30" t="s">
-        <v>30</v>
-      </c>
-      <c r="O30" t="s">
-        <v>30</v>
-      </c>
-      <c r="P30" t="s">
-        <v>30</v>
-      </c>
       <c r="Q30" t="s">
         <v>30</v>
       </c>
       <c r="R30" t="s">
-        <v>31</v>
+        <v>155</v>
       </c>
       <c r="T30" t="s">
         <v>30</v>
       </c>
       <c r="W30" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="X30" s="12" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>158</v>
       </c>
-      <c r="C31" t="s">
+      <c r="B31" t="s">
         <v>159</v>
       </c>
       <c r="F31">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="K31" t="s">
         <v>30</v>
@@ -2563,39 +2551,45 @@
       <c r="L31" t="s">
         <v>30</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="O31" t="s">
+        <v>30</v>
+      </c>
+      <c r="P31" t="s">
         <v>30</v>
       </c>
       <c r="R31" t="s">
+        <v>31</v>
+      </c>
+      <c r="T31" t="s">
+        <v>30</v>
+      </c>
+      <c r="W31" t="s">
         <v>160</v>
       </c>
-      <c r="T31" t="s">
-        <v>30</v>
-      </c>
-      <c r="W31" t="s">
+      <c r="X31" s="12" t="s">
         <v>161</v>
-      </c>
-      <c r="X31" s="12" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>162</v>
+      </c>
+      <c r="B32" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="B32" t="s">
-        <v>164</v>
-      </c>
       <c r="F32">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G32">
-        <v>10</v>
+        <v>100</v>
+      </c>
+      <c r="J32" t="s">
+        <v>30</v>
       </c>
       <c r="K32" t="s">
         <v>30</v>
       </c>
-      <c r="L32" t="s">
+      <c r="N32" t="s">
         <v>30</v>
       </c>
       <c r="O32" t="s">
@@ -2611,83 +2605,42 @@
         <v>30</v>
       </c>
       <c r="W32" t="s">
+        <v>164</v>
+      </c>
+      <c r="X32" t="s">
         <v>165</v>
-      </c>
-      <c r="X32" s="12" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>166</v>
+      </c>
+      <c r="B33" t="s">
         <v>167</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="C33" t="s">
         <v>168</v>
       </c>
+      <c r="D33" t="s">
+        <v>169</v>
+      </c>
       <c r="F33">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G33">
-        <v>100</v>
-      </c>
-      <c r="J33" t="s">
-        <v>30</v>
-      </c>
-      <c r="K33" t="s">
-        <v>30</v>
-      </c>
-      <c r="N33" t="s">
-        <v>30</v>
-      </c>
-      <c r="O33" t="s">
-        <v>30</v>
-      </c>
-      <c r="P33" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="R33" t="s">
-        <v>31</v>
+        <v>170</v>
       </c>
       <c r="T33" t="s">
         <v>30</v>
       </c>
       <c r="W33" t="s">
-        <v>169</v>
-      </c>
-      <c r="X33" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
         <v>171</v>
       </c>
-      <c r="B34" t="s">
+      <c r="X33" s="12" t="s">
         <v>172</v>
-      </c>
-      <c r="C34" t="s">
-        <v>173</v>
-      </c>
-      <c r="D34" t="s">
-        <v>174</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <v>10</v>
-      </c>
-      <c r="R34" t="s">
-        <v>175</v>
-      </c>
-      <c r="T34" t="s">
-        <v>30</v>
-      </c>
-      <c r="W34" t="s">
-        <v>176</v>
-      </c>
-      <c r="X34" s="12" t="s">
-        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2700,7 +2653,7 @@
     <mergeCell ref="R1:S1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B33" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B32" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
update manufacturer structure to include notice field
</commit_message>
<xml_diff>
--- a/data/atr_data.xlsx
+++ b/data/atr_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pp-brandon/Projects/uiowa-atr/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0472EE8-5DBB-C44A-B044-C7676E906E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA53CA56-58D8-C445-B492-7B7B9399F68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="183">
   <si>
     <t>Resource:</t>
   </si>
@@ -645,12 +645,58 @@
   <si>
     <t>ENVIRONMENT</t>
   </si>
+  <si>
+    <t>notice</t>
+  </si>
+  <si>
+    <r>
+      <t>The clinician needs to have a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>clinician account</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> and provide the user with a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>join code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t> to use this resource.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -688,6 +734,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="18">
@@ -841,7 +900,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1225,10 +1284,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X33"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1247,13 +1306,13 @@
     <col min="17" max="17" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="21.33203125" customWidth="1"/>
     <col min="19" max="19" width="8.6640625" customWidth="1"/>
-    <col min="20" max="20" width="11.6640625" customWidth="1"/>
+    <col min="20" max="20" width="92.1640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="23.33203125" customWidth="1"/>
     <col min="23" max="23" width="29" customWidth="1"/>
     <col min="24" max="24" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1281,23 +1340,24 @@
       </c>
       <c r="P1" s="20"/>
       <c r="Q1" s="20"/>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="21"/>
-      <c r="T1" s="16" t="s">
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="U1" s="16"/>
       <c r="V1" s="16"/>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="16"/>
+      <c r="X1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -1355,23 +1415,26 @@
       <c r="S2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="T2" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="U2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="X2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="Y2" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1402,17 +1465,17 @@
       <c r="R3" t="s">
         <v>31</v>
       </c>
-      <c r="T3" t="s">
-        <v>30</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="U3" t="s">
+        <v>30</v>
+      </c>
+      <c r="X3" t="s">
         <v>32</v>
       </c>
-      <c r="X3" s="12" t="s">
+      <c r="Y3" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1446,17 +1509,17 @@
       <c r="R4" t="s">
         <v>173</v>
       </c>
-      <c r="T4" t="s">
-        <v>30</v>
-      </c>
-      <c r="W4" t="s">
+      <c r="U4" t="s">
+        <v>30</v>
+      </c>
+      <c r="X4" t="s">
         <v>37</v>
       </c>
-      <c r="X4" s="12" t="s">
+      <c r="Y4" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1487,17 +1550,20 @@
       <c r="R5" t="s">
         <v>39</v>
       </c>
-      <c r="U5" t="s">
-        <v>30</v>
-      </c>
-      <c r="W5" t="s">
+      <c r="T5" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="V5" t="s">
+        <v>30</v>
+      </c>
+      <c r="X5" t="s">
         <v>41</v>
       </c>
-      <c r="X5" s="12" t="s">
+      <c r="Y5" s="12" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1531,17 +1597,17 @@
       <c r="R6" t="s">
         <v>45</v>
       </c>
-      <c r="T6" t="s">
-        <v>30</v>
-      </c>
-      <c r="W6" t="s">
+      <c r="U6" t="s">
+        <v>30</v>
+      </c>
+      <c r="X6" t="s">
         <v>46</v>
       </c>
-      <c r="X6" s="12" t="s">
+      <c r="Y6" s="12" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -1572,17 +1638,17 @@
       <c r="R7" t="s">
         <v>50</v>
       </c>
-      <c r="T7" t="s">
-        <v>30</v>
-      </c>
-      <c r="W7" t="s">
+      <c r="U7" t="s">
+        <v>30</v>
+      </c>
+      <c r="X7" t="s">
         <v>51</v>
       </c>
-      <c r="X7" s="12" t="s">
+      <c r="Y7" s="12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1613,17 +1679,17 @@
       <c r="R8" t="s">
         <v>55</v>
       </c>
-      <c r="T8" t="s">
-        <v>30</v>
-      </c>
-      <c r="W8" t="s">
+      <c r="U8" t="s">
+        <v>30</v>
+      </c>
+      <c r="X8" t="s">
         <v>56</v>
       </c>
-      <c r="X8" s="12" t="s">
+      <c r="Y8" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -1651,20 +1717,20 @@
       <c r="R9" t="s">
         <v>62</v>
       </c>
-      <c r="T9" t="s">
-        <v>30</v>
-      </c>
       <c r="U9" t="s">
         <v>30</v>
       </c>
-      <c r="W9" t="s">
+      <c r="V9" t="s">
+        <v>30</v>
+      </c>
+      <c r="X9" t="s">
         <v>63</v>
       </c>
-      <c r="X9" s="12" t="s">
+      <c r="Y9" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1692,17 +1758,17 @@
       <c r="R10" t="s">
         <v>31</v>
       </c>
-      <c r="T10" t="s">
-        <v>30</v>
-      </c>
-      <c r="W10" t="s">
+      <c r="U10" t="s">
+        <v>30</v>
+      </c>
+      <c r="X10" t="s">
         <v>68</v>
       </c>
-      <c r="X10" s="12" t="s">
+      <c r="Y10" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -1728,17 +1794,17 @@
         <v>177</v>
       </c>
       <c r="S11" s="13"/>
-      <c r="T11" t="s">
-        <v>30</v>
-      </c>
-      <c r="W11" t="s">
+      <c r="U11" t="s">
+        <v>30</v>
+      </c>
+      <c r="X11" t="s">
         <v>72</v>
       </c>
-      <c r="X11" s="12" t="s">
+      <c r="Y11" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -1769,17 +1835,17 @@
       <c r="S12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="T12" t="s">
-        <v>30</v>
-      </c>
-      <c r="W12" t="s">
+      <c r="U12" t="s">
+        <v>30</v>
+      </c>
+      <c r="X12" t="s">
         <v>77</v>
       </c>
-      <c r="X12" s="14" t="s">
+      <c r="Y12" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -1816,17 +1882,17 @@
       <c r="S13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="T13" t="s">
-        <v>30</v>
-      </c>
-      <c r="W13" t="s">
+      <c r="U13" t="s">
+        <v>30</v>
+      </c>
+      <c r="X13" t="s">
         <v>81</v>
       </c>
-      <c r="X13" s="14" t="s">
+      <c r="Y13" s="14" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -1875,17 +1941,17 @@
       <c r="R14" t="s">
         <v>86</v>
       </c>
-      <c r="T14" t="s">
-        <v>30</v>
-      </c>
-      <c r="W14" t="s">
+      <c r="U14" t="s">
+        <v>30</v>
+      </c>
+      <c r="X14" t="s">
         <v>87</v>
       </c>
-      <c r="X14" s="14" t="s">
+      <c r="Y14" s="14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -1919,20 +1985,20 @@
       <c r="R15" t="s">
         <v>92</v>
       </c>
-      <c r="T15" t="s">
-        <v>30</v>
-      </c>
       <c r="U15" t="s">
         <v>30</v>
       </c>
-      <c r="W15" t="s">
+      <c r="V15" t="s">
+        <v>30</v>
+      </c>
+      <c r="X15" t="s">
         <v>93</v>
       </c>
-      <c r="X15" s="12" t="s">
+      <c r="Y15" s="12" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -1963,17 +2029,17 @@
       <c r="R16" t="s">
         <v>97</v>
       </c>
-      <c r="U16" t="s">
-        <v>30</v>
-      </c>
-      <c r="W16" t="s">
+      <c r="V16" t="s">
+        <v>30</v>
+      </c>
+      <c r="X16" t="s">
         <v>98</v>
       </c>
-      <c r="X16" s="12" t="s">
+      <c r="Y16" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>100</v>
       </c>
@@ -1998,17 +2064,17 @@
       <c r="R17" t="s">
         <v>173</v>
       </c>
-      <c r="U17" t="s">
-        <v>30</v>
-      </c>
-      <c r="W17" t="s">
+      <c r="V17" t="s">
+        <v>30</v>
+      </c>
+      <c r="X17" t="s">
         <v>37</v>
       </c>
-      <c r="X17" s="12" t="s">
+      <c r="Y17" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -2039,17 +2105,17 @@
       <c r="R18" t="s">
         <v>103</v>
       </c>
-      <c r="U18" t="s">
-        <v>30</v>
-      </c>
-      <c r="W18" t="s">
+      <c r="V18" t="s">
+        <v>30</v>
+      </c>
+      <c r="X18" t="s">
         <v>105</v>
       </c>
-      <c r="X18" s="12" t="s">
+      <c r="Y18" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>107</v>
       </c>
@@ -2074,17 +2140,17 @@
       <c r="R19" t="s">
         <v>109</v>
       </c>
-      <c r="T19" t="s">
-        <v>30</v>
-      </c>
-      <c r="W19" t="s">
+      <c r="U19" t="s">
+        <v>30</v>
+      </c>
+      <c r="X19" t="s">
         <v>110</v>
       </c>
-      <c r="X19" s="12" t="s">
+      <c r="Y19" s="12" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>112</v>
       </c>
@@ -2112,17 +2178,17 @@
       <c r="R20" t="s">
         <v>55</v>
       </c>
-      <c r="T20" t="s">
-        <v>30</v>
-      </c>
-      <c r="W20" t="s">
+      <c r="U20" t="s">
+        <v>30</v>
+      </c>
+      <c r="X20" t="s">
         <v>56</v>
       </c>
-      <c r="X20" s="12" t="s">
+      <c r="Y20" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>115</v>
       </c>
@@ -2153,17 +2219,17 @@
       <c r="R21" t="s">
         <v>118</v>
       </c>
-      <c r="T21" t="s">
-        <v>30</v>
-      </c>
-      <c r="W21" t="s">
+      <c r="U21" t="s">
+        <v>30</v>
+      </c>
+      <c r="X21" t="s">
         <v>119</v>
       </c>
-      <c r="X21" s="12" t="s">
+      <c r="Y21" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>121</v>
       </c>
@@ -2185,14 +2251,14 @@
       <c r="R22" t="s">
         <v>123</v>
       </c>
-      <c r="W22" t="s">
+      <c r="X22" t="s">
         <v>124</v>
       </c>
-      <c r="X22" s="12" t="s">
+      <c r="Y22" s="12" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -2220,17 +2286,17 @@
       <c r="R23" t="s">
         <v>31</v>
       </c>
-      <c r="T23" t="s">
-        <v>30</v>
-      </c>
-      <c r="W23" t="s">
+      <c r="U23" t="s">
+        <v>30</v>
+      </c>
+      <c r="X23" t="s">
         <v>128</v>
       </c>
-      <c r="X23" s="12" t="s">
+      <c r="Y23" s="12" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -2264,17 +2330,17 @@
       <c r="R24" t="s">
         <v>131</v>
       </c>
-      <c r="U24" t="s">
-        <v>30</v>
-      </c>
-      <c r="W24" t="s">
+      <c r="V24" t="s">
+        <v>30</v>
+      </c>
+      <c r="X24" t="s">
         <v>178</v>
       </c>
-      <c r="X24" s="12" t="s">
+      <c r="Y24" s="12" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>133</v>
       </c>
@@ -2314,20 +2380,20 @@
       <c r="R25" t="s">
         <v>135</v>
       </c>
-      <c r="T25" t="s">
-        <v>30</v>
-      </c>
       <c r="U25" t="s">
         <v>30</v>
       </c>
-      <c r="W25" t="s">
+      <c r="V25" t="s">
+        <v>30</v>
+      </c>
+      <c r="X25" t="s">
         <v>136</v>
       </c>
-      <c r="X25" s="14" t="s">
+      <c r="Y25" s="14" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -2352,20 +2418,20 @@
       <c r="R26" t="s">
         <v>138</v>
       </c>
-      <c r="T26" t="s">
-        <v>30</v>
-      </c>
       <c r="U26" t="s">
         <v>30</v>
       </c>
-      <c r="W26" t="s">
+      <c r="V26" t="s">
+        <v>30</v>
+      </c>
+      <c r="X26" t="s">
         <v>142</v>
       </c>
-      <c r="X26" s="12" t="s">
+      <c r="Y26" s="12" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>144</v>
       </c>
@@ -2399,17 +2465,17 @@
       <c r="R27" t="s">
         <v>31</v>
       </c>
-      <c r="T27" t="s">
-        <v>30</v>
-      </c>
-      <c r="W27" t="s">
+      <c r="U27" t="s">
+        <v>30</v>
+      </c>
+      <c r="X27" t="s">
         <v>128</v>
       </c>
-      <c r="X27" s="12" t="s">
+      <c r="Y27" s="12" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -2437,17 +2503,17 @@
       <c r="R28" t="s">
         <v>148</v>
       </c>
-      <c r="T28" t="s">
-        <v>30</v>
-      </c>
-      <c r="W28" t="s">
+      <c r="U28" t="s">
+        <v>30</v>
+      </c>
+      <c r="X28" t="s">
         <v>149</v>
       </c>
-      <c r="X28" s="12" t="s">
+      <c r="Y28" s="12" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>151</v>
       </c>
@@ -2487,17 +2553,17 @@
       <c r="R29" t="s">
         <v>31</v>
       </c>
-      <c r="T29" t="s">
-        <v>30</v>
-      </c>
-      <c r="W29" t="s">
+      <c r="U29" t="s">
+        <v>30</v>
+      </c>
+      <c r="X29" t="s">
         <v>128</v>
       </c>
-      <c r="X29" s="12" t="s">
+      <c r="Y29" s="12" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>153</v>
       </c>
@@ -2522,17 +2588,17 @@
       <c r="R30" t="s">
         <v>155</v>
       </c>
-      <c r="T30" t="s">
-        <v>30</v>
-      </c>
-      <c r="W30" t="s">
+      <c r="U30" t="s">
+        <v>30</v>
+      </c>
+      <c r="X30" t="s">
         <v>156</v>
       </c>
-      <c r="X30" s="12" t="s">
+      <c r="Y30" s="12" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>158</v>
       </c>
@@ -2560,17 +2626,17 @@
       <c r="R31" t="s">
         <v>31</v>
       </c>
-      <c r="T31" t="s">
-        <v>30</v>
-      </c>
-      <c r="W31" t="s">
+      <c r="U31" t="s">
+        <v>30</v>
+      </c>
+      <c r="X31" t="s">
         <v>160</v>
       </c>
-      <c r="X31" s="12" t="s">
+      <c r="Y31" s="12" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>162</v>
       </c>
@@ -2601,17 +2667,17 @@
       <c r="R32" t="s">
         <v>31</v>
       </c>
-      <c r="T32" t="s">
-        <v>30</v>
-      </c>
-      <c r="W32" t="s">
+      <c r="U32" t="s">
+        <v>30</v>
+      </c>
+      <c r="X32" t="s">
         <v>164</v>
       </c>
-      <c r="X32" t="s">
+      <c r="Y32" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>166</v>
       </c>
@@ -2633,24 +2699,24 @@
       <c r="R33" t="s">
         <v>170</v>
       </c>
-      <c r="T33" t="s">
-        <v>30</v>
-      </c>
-      <c r="W33" t="s">
+      <c r="U33" t="s">
+        <v>30</v>
+      </c>
+      <c r="X33" t="s">
         <v>171</v>
       </c>
-      <c r="X33" s="12" t="s">
+      <c r="Y33" s="12" t="s">
         <v>172</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="T1:V1"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:N1"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="R1:T1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B32" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>

</xml_diff>